<commit_message>
added ML bin and poi, fixed taz2cell20 but not final
</commit_message>
<xml_diff>
--- a/Data/division_choice/20/taz2cell.xlsx
+++ b/Data/division_choice/20/taz2cell.xlsx
@@ -2,24 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\חיל אוויר\קורונה\Code\SEIR_model\Data\division_choice\20\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="1560" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="taz2cell" sheetId="1" r:id="rId1"/>
+    <sheet name="taz2area_code" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="6">
   <si>
     <t>51_tlv</t>
   </si>
@@ -49,6 +49,7 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -56,6 +57,7 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -63,6 +65,7 @@
       <color theme="3"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -71,6 +74,7 @@
       <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -79,6 +83,7 @@
       <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -87,6 +92,7 @@
       <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -94,6 +100,7 @@
       <color rgb="FF006100"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -101,13 +108,15 @@
       <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -115,6 +124,7 @@
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,6 +133,7 @@
       <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -131,6 +142,7 @@
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,6 +150,7 @@
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -146,6 +159,7 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,6 +167,7 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,6 +176,7 @@
       <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -169,6 +185,7 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -176,6 +193,7 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -498,27 +516,27 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -597,7 +615,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -609,7 +627,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -656,23 +674,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -708,23 +709,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -879,14 +863,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2631"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -900,8 +881,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -924,8 +905,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>43</v>
+      <c r="B5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3085,7 +3066,7 @@
         <v>274</v>
       </c>
       <c r="B275">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
@@ -3093,7 +3074,7 @@
         <v>275</v>
       </c>
       <c r="B276">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
@@ -3101,7 +3082,7 @@
         <v>276</v>
       </c>
       <c r="B277">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
@@ -3205,7 +3186,7 @@
         <v>289</v>
       </c>
       <c r="B290">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
@@ -3213,7 +3194,7 @@
         <v>290</v>
       </c>
       <c r="B291">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
@@ -3221,7 +3202,7 @@
         <v>291</v>
       </c>
       <c r="B292">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
@@ -3701,7 +3682,7 @@
         <v>351</v>
       </c>
       <c r="B352">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
@@ -3709,7 +3690,7 @@
         <v>352</v>
       </c>
       <c r="B353">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
@@ -3717,7 +3698,7 @@
         <v>353</v>
       </c>
       <c r="B354">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
@@ -4573,7 +4554,7 @@
         <v>460</v>
       </c>
       <c r="B461">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
@@ -4581,7 +4562,7 @@
         <v>461</v>
       </c>
       <c r="B462">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
@@ -4589,7 +4570,7 @@
         <v>462</v>
       </c>
       <c r="B463">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
@@ -4629,7 +4610,7 @@
         <v>467</v>
       </c>
       <c r="B468">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
@@ -4797,7 +4778,7 @@
         <v>488</v>
       </c>
       <c r="B489">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.2">
@@ -4805,7 +4786,7 @@
         <v>489</v>
       </c>
       <c r="B490">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
@@ -4813,7 +4794,7 @@
         <v>490</v>
       </c>
       <c r="B491">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
@@ -4917,7 +4898,7 @@
         <v>503</v>
       </c>
       <c r="B504">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
@@ -4925,7 +4906,7 @@
         <v>504</v>
       </c>
       <c r="B505">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
@@ -4933,7 +4914,7 @@
         <v>505</v>
       </c>
       <c r="B506">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
@@ -4973,7 +4954,7 @@
         <v>510</v>
       </c>
       <c r="B511">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
@@ -4981,7 +4962,7 @@
         <v>511</v>
       </c>
       <c r="B512">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
@@ -4989,7 +4970,7 @@
         <v>512</v>
       </c>
       <c r="B513">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
@@ -5749,7 +5730,7 @@
         <v>607</v>
       </c>
       <c r="B608">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
@@ -5757,7 +5738,7 @@
         <v>608</v>
       </c>
       <c r="B609">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
@@ -5765,7 +5746,7 @@
         <v>609</v>
       </c>
       <c r="B610">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
@@ -5901,7 +5882,7 @@
         <v>626</v>
       </c>
       <c r="B627">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
@@ -5909,7 +5890,7 @@
         <v>627</v>
       </c>
       <c r="B628">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
@@ -5917,7 +5898,7 @@
         <v>628</v>
       </c>
       <c r="B629">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
@@ -6117,7 +6098,7 @@
         <v>653</v>
       </c>
       <c r="B654">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
@@ -6125,7 +6106,7 @@
         <v>654</v>
       </c>
       <c r="B655">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
@@ -6133,7 +6114,7 @@
         <v>655</v>
       </c>
       <c r="B656">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
@@ -6557,7 +6538,7 @@
         <v>708</v>
       </c>
       <c r="B709">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
@@ -6565,7 +6546,7 @@
         <v>709</v>
       </c>
       <c r="B710">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
@@ -6573,7 +6554,7 @@
         <v>710</v>
       </c>
       <c r="B711">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
@@ -6709,7 +6690,7 @@
         <v>727</v>
       </c>
       <c r="B728">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
@@ -6717,7 +6698,7 @@
         <v>728</v>
       </c>
       <c r="B729">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
@@ -6725,7 +6706,7 @@
         <v>729</v>
       </c>
       <c r="B730">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
@@ -6917,7 +6898,7 @@
         <v>753</v>
       </c>
       <c r="B754">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
@@ -6925,7 +6906,7 @@
         <v>754</v>
       </c>
       <c r="B755">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.2">
@@ -6933,7 +6914,7 @@
         <v>755</v>
       </c>
       <c r="B756">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
@@ -7221,7 +7202,7 @@
         <v>791</v>
       </c>
       <c r="B792">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.2">
@@ -7229,7 +7210,7 @@
         <v>792</v>
       </c>
       <c r="B793">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.2">
@@ -7237,7 +7218,7 @@
         <v>793</v>
       </c>
       <c r="B794">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.2">
@@ -7469,7 +7450,7 @@
         <v>822</v>
       </c>
       <c r="B823">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
@@ -7477,7 +7458,7 @@
         <v>823</v>
       </c>
       <c r="B824">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
@@ -7485,7 +7466,7 @@
         <v>824</v>
       </c>
       <c r="B825">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
@@ -7925,7 +7906,7 @@
         <v>879</v>
       </c>
       <c r="B880">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
@@ -7933,7 +7914,7 @@
         <v>880</v>
       </c>
       <c r="B881">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
@@ -7941,7 +7922,7 @@
         <v>881</v>
       </c>
       <c r="B882">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
@@ -8141,7 +8122,7 @@
         <v>906</v>
       </c>
       <c r="B907">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
@@ -8165,7 +8146,7 @@
         <v>909</v>
       </c>
       <c r="B910">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
@@ -8205,7 +8186,7 @@
         <v>914</v>
       </c>
       <c r="B915">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
@@ -8213,7 +8194,7 @@
         <v>915</v>
       </c>
       <c r="B916">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
@@ -8221,7 +8202,7 @@
         <v>916</v>
       </c>
       <c r="B917">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
@@ -8357,7 +8338,7 @@
         <v>933</v>
       </c>
       <c r="B934">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
@@ -8381,7 +8362,7 @@
         <v>936</v>
       </c>
       <c r="B937">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
@@ -8405,7 +8386,7 @@
         <v>939</v>
       </c>
       <c r="B940">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
@@ -8413,7 +8394,7 @@
         <v>940</v>
       </c>
       <c r="B941">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
@@ -8421,7 +8402,7 @@
         <v>941</v>
       </c>
       <c r="B942">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
@@ -8565,7 +8546,7 @@
         <v>959</v>
       </c>
       <c r="B960">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
@@ -8573,7 +8554,7 @@
         <v>960</v>
       </c>
       <c r="B961">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
@@ -8581,7 +8562,7 @@
         <v>961</v>
       </c>
       <c r="B962">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
@@ -8597,7 +8578,7 @@
         <v>963</v>
       </c>
       <c r="B964">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
@@ -8605,7 +8586,7 @@
         <v>964</v>
       </c>
       <c r="B965">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
@@ -8613,7 +8594,7 @@
         <v>965</v>
       </c>
       <c r="B966">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
@@ -8717,7 +8698,7 @@
         <v>978</v>
       </c>
       <c r="B979">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
@@ -8725,7 +8706,7 @@
         <v>979</v>
       </c>
       <c r="B980">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
@@ -8733,7 +8714,7 @@
         <v>980</v>
       </c>
       <c r="B981">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
@@ -8789,7 +8770,7 @@
         <v>987</v>
       </c>
       <c r="B988">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
@@ -8797,7 +8778,7 @@
         <v>988</v>
       </c>
       <c r="B989">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
@@ -8805,7 +8786,7 @@
         <v>989</v>
       </c>
       <c r="B990">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
@@ -8845,7 +8826,7 @@
         <v>994</v>
       </c>
       <c r="B995">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
@@ -8861,7 +8842,7 @@
         <v>996</v>
       </c>
       <c r="B997">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
@@ -8869,7 +8850,7 @@
         <v>997</v>
       </c>
       <c r="B998">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
@@ -8877,7 +8858,7 @@
         <v>998</v>
       </c>
       <c r="B999">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
@@ -9069,7 +9050,7 @@
         <v>1022</v>
       </c>
       <c r="B1023">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
@@ -9077,7 +9058,7 @@
         <v>1023</v>
       </c>
       <c r="B1024">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
@@ -9085,7 +9066,7 @@
         <v>1024</v>
       </c>
       <c r="B1025">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
@@ -9101,7 +9082,7 @@
         <v>1026</v>
       </c>
       <c r="B1027">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
@@ -9109,7 +9090,7 @@
         <v>1027</v>
       </c>
       <c r="B1028">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
@@ -9117,7 +9098,7 @@
         <v>1028</v>
       </c>
       <c r="B1029">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
@@ -9157,7 +9138,7 @@
         <v>1033</v>
       </c>
       <c r="B1034">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
@@ -9165,7 +9146,7 @@
         <v>1034</v>
       </c>
       <c r="B1035">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
@@ -9173,7 +9154,7 @@
         <v>1035</v>
       </c>
       <c r="B1036">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
@@ -9196,24 +9177,24 @@
       <c r="A1039">
         <v>1038</v>
       </c>
-      <c r="B1039">
-        <v>43</v>
+      <c r="B1039" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040">
         <v>1039</v>
       </c>
-      <c r="B1040">
-        <v>43</v>
+      <c r="B1040" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041">
         <v>1040</v>
       </c>
-      <c r="B1041">
-        <v>43</v>
+      <c r="B1041" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
@@ -9221,7 +9202,7 @@
         <v>1041</v>
       </c>
       <c r="B1042">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
@@ -9229,7 +9210,7 @@
         <v>1042</v>
       </c>
       <c r="B1043">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
@@ -9237,7 +9218,7 @@
         <v>1043</v>
       </c>
       <c r="B1044">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
@@ -9245,7 +9226,7 @@
         <v>1044</v>
       </c>
       <c r="B1045">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
@@ -9253,7 +9234,7 @@
         <v>1045</v>
       </c>
       <c r="B1046">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
@@ -9261,7 +9242,7 @@
         <v>1046</v>
       </c>
       <c r="B1047">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
@@ -9269,7 +9250,7 @@
         <v>1047</v>
       </c>
       <c r="B1048">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
@@ -9277,7 +9258,7 @@
         <v>1048</v>
       </c>
       <c r="B1049">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
@@ -11165,7 +11146,7 @@
         <v>1284</v>
       </c>
       <c r="B1285">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1286" spans="1:2" x14ac:dyDescent="0.2">
@@ -11173,7 +11154,7 @@
         <v>1285</v>
       </c>
       <c r="B1286">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1287" spans="1:2" x14ac:dyDescent="0.2">
@@ -11181,7 +11162,7 @@
         <v>1286</v>
       </c>
       <c r="B1287">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1288" spans="1:2" x14ac:dyDescent="0.2">
@@ -11325,7 +11306,7 @@
         <v>1304</v>
       </c>
       <c r="B1305">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1306" spans="1:2" x14ac:dyDescent="0.2">
@@ -11333,7 +11314,7 @@
         <v>1305</v>
       </c>
       <c r="B1306">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1307" spans="1:2" x14ac:dyDescent="0.2">
@@ -11341,7 +11322,7 @@
         <v>1306</v>
       </c>
       <c r="B1307">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1308" spans="1:2" x14ac:dyDescent="0.2">
@@ -11453,7 +11434,7 @@
         <v>1320</v>
       </c>
       <c r="B1321">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1322" spans="1:2" x14ac:dyDescent="0.2">
@@ -11461,7 +11442,7 @@
         <v>1321</v>
       </c>
       <c r="B1322">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1323" spans="1:2" x14ac:dyDescent="0.2">
@@ -11469,7 +11450,7 @@
         <v>1322</v>
       </c>
       <c r="B1323">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1324" spans="1:2" x14ac:dyDescent="0.2">
@@ -11876,24 +11857,24 @@
       <c r="A1374">
         <v>1373</v>
       </c>
-      <c r="B1374">
-        <v>71</v>
+      <c r="B1374" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1375">
         <v>1374</v>
       </c>
-      <c r="B1375">
-        <v>71</v>
+      <c r="B1375" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1376">
         <v>1375</v>
       </c>
-      <c r="B1376">
-        <v>71</v>
+      <c r="B1376" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1377" spans="1:2" x14ac:dyDescent="0.2">
@@ -11956,8 +11937,8 @@
       <c r="A1384">
         <v>1383</v>
       </c>
-      <c r="B1384">
-        <v>11</v>
+      <c r="B1384" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="1385" spans="1:2" x14ac:dyDescent="0.2">
@@ -12429,7 +12410,7 @@
         <v>1442</v>
       </c>
       <c r="B1443">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1444" spans="1:2" x14ac:dyDescent="0.2">
@@ -12437,7 +12418,7 @@
         <v>1443</v>
       </c>
       <c r="B1444">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1445" spans="1:2" x14ac:dyDescent="0.2">
@@ -12469,7 +12450,7 @@
         <v>1447</v>
       </c>
       <c r="B1448">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1449" spans="1:2" x14ac:dyDescent="0.2">
@@ -12709,7 +12690,7 @@
         <v>1477</v>
       </c>
       <c r="B1478">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1479" spans="1:2" x14ac:dyDescent="0.2">
@@ -12717,7 +12698,7 @@
         <v>1478</v>
       </c>
       <c r="B1479">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1480" spans="1:2" x14ac:dyDescent="0.2">
@@ -12725,7 +12706,7 @@
         <v>1479</v>
       </c>
       <c r="B1480">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1481" spans="1:2" x14ac:dyDescent="0.2">
@@ -12837,7 +12818,7 @@
         <v>1493</v>
       </c>
       <c r="B1494">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1495" spans="1:2" x14ac:dyDescent="0.2">
@@ -12845,7 +12826,7 @@
         <v>1494</v>
       </c>
       <c r="B1495">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1496" spans="1:2" x14ac:dyDescent="0.2">
@@ -12853,7 +12834,7 @@
         <v>1495</v>
       </c>
       <c r="B1496">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1497" spans="1:2" x14ac:dyDescent="0.2">
@@ -13277,7 +13258,7 @@
         <v>1548</v>
       </c>
       <c r="B1549">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1550" spans="1:2" x14ac:dyDescent="0.2">
@@ -13285,7 +13266,7 @@
         <v>1549</v>
       </c>
       <c r="B1550">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1551" spans="1:2" x14ac:dyDescent="0.2">
@@ -13293,7 +13274,7 @@
         <v>1550</v>
       </c>
       <c r="B1551">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1552" spans="1:2" x14ac:dyDescent="0.2">
@@ -13333,7 +13314,7 @@
         <v>1555</v>
       </c>
       <c r="B1556">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1557" spans="1:2" x14ac:dyDescent="0.2">
@@ -13349,7 +13330,7 @@
         <v>1557</v>
       </c>
       <c r="B1558">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1559" spans="1:2" x14ac:dyDescent="0.2">
@@ -13365,7 +13346,7 @@
         <v>1559</v>
       </c>
       <c r="B1560">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="1561" spans="1:2" x14ac:dyDescent="0.2">
@@ -14229,7 +14210,7 @@
         <v>1667</v>
       </c>
       <c r="B1668">
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1669" spans="1:2" x14ac:dyDescent="0.2">
@@ -14237,7 +14218,7 @@
         <v>1668</v>
       </c>
       <c r="B1669">
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1670" spans="1:2" x14ac:dyDescent="0.2">
@@ -14245,7 +14226,7 @@
         <v>1669</v>
       </c>
       <c r="B1670">
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1671" spans="1:2" x14ac:dyDescent="0.2">
@@ -15085,7 +15066,7 @@
         <v>1774</v>
       </c>
       <c r="B1775">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1776" spans="1:2" x14ac:dyDescent="0.2">
@@ -15093,7 +15074,7 @@
         <v>1775</v>
       </c>
       <c r="B1776">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1777" spans="1:2" x14ac:dyDescent="0.2">
@@ -15413,7 +15394,7 @@
         <v>1815</v>
       </c>
       <c r="B1816">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1817" spans="1:2" x14ac:dyDescent="0.2">
@@ -15437,7 +15418,7 @@
         <v>1818</v>
       </c>
       <c r="B1819">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1820" spans="1:2" x14ac:dyDescent="0.2">
@@ -15653,7 +15634,7 @@
         <v>1845</v>
       </c>
       <c r="B1846">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1847" spans="1:2" x14ac:dyDescent="0.2">
@@ -15677,7 +15658,7 @@
         <v>1848</v>
       </c>
       <c r="B1849">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1850" spans="1:2" x14ac:dyDescent="0.2">
@@ -15717,7 +15698,7 @@
         <v>1853</v>
       </c>
       <c r="B1854">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1855" spans="1:2" x14ac:dyDescent="0.2">
@@ -15725,7 +15706,7 @@
         <v>1854</v>
       </c>
       <c r="B1855">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1856" spans="1:2" x14ac:dyDescent="0.2">
@@ -15733,7 +15714,7 @@
         <v>1855</v>
       </c>
       <c r="B1856">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="1857" spans="1:2" x14ac:dyDescent="0.2">
@@ -15861,7 +15842,7 @@
         <v>1871</v>
       </c>
       <c r="B1872">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1873" spans="1:2" x14ac:dyDescent="0.2">
@@ -15869,7 +15850,7 @@
         <v>1872</v>
       </c>
       <c r="B1873">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1874" spans="1:2" x14ac:dyDescent="0.2">
@@ -15877,7 +15858,7 @@
         <v>1873</v>
       </c>
       <c r="B1874">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1875" spans="1:2" x14ac:dyDescent="0.2">
@@ -15917,7 +15898,7 @@
         <v>1878</v>
       </c>
       <c r="B1879">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1880" spans="1:2" x14ac:dyDescent="0.2">
@@ -15925,7 +15906,7 @@
         <v>1879</v>
       </c>
       <c r="B1880">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1881" spans="1:2" x14ac:dyDescent="0.2">
@@ -15933,7 +15914,7 @@
         <v>1880</v>
       </c>
       <c r="B1881">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1882" spans="1:2" x14ac:dyDescent="0.2">
@@ -15989,7 +15970,7 @@
         <v>1887</v>
       </c>
       <c r="B1888">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1889" spans="1:2" x14ac:dyDescent="0.2">
@@ -16013,7 +15994,7 @@
         <v>1890</v>
       </c>
       <c r="B1891">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1892" spans="1:2" x14ac:dyDescent="0.2">
@@ -16045,7 +16026,7 @@
         <v>1894</v>
       </c>
       <c r="B1895">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1896" spans="1:2" x14ac:dyDescent="0.2">
@@ -16053,7 +16034,7 @@
         <v>1895</v>
       </c>
       <c r="B1896">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1897" spans="1:2" x14ac:dyDescent="0.2">
@@ -16061,7 +16042,7 @@
         <v>1896</v>
       </c>
       <c r="B1897">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1898" spans="1:2" x14ac:dyDescent="0.2">
@@ -16493,7 +16474,7 @@
         <v>1950</v>
       </c>
       <c r="B1951">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1952" spans="1:2" x14ac:dyDescent="0.2">
@@ -16501,7 +16482,7 @@
         <v>1951</v>
       </c>
       <c r="B1952">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1953" spans="1:2" x14ac:dyDescent="0.2">
@@ -16509,7 +16490,7 @@
         <v>1952</v>
       </c>
       <c r="B1953">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1954" spans="1:2" x14ac:dyDescent="0.2">
@@ -16941,7 +16922,7 @@
         <v>2006</v>
       </c>
       <c r="B2007">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2008" spans="1:2" x14ac:dyDescent="0.2">
@@ -16965,7 +16946,7 @@
         <v>2009</v>
       </c>
       <c r="B2010">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2011" spans="1:2" x14ac:dyDescent="0.2">
@@ -17629,7 +17610,7 @@
         <v>2092</v>
       </c>
       <c r="B2093">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2094" spans="1:2" x14ac:dyDescent="0.2">
@@ -17661,7 +17642,7 @@
         <v>2096</v>
       </c>
       <c r="B2097">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2098" spans="1:2" x14ac:dyDescent="0.2">
@@ -17677,7 +17658,7 @@
         <v>2098</v>
       </c>
       <c r="B2099">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2100" spans="1:2" x14ac:dyDescent="0.2">
@@ -17685,7 +17666,7 @@
         <v>2099</v>
       </c>
       <c r="B2100">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2101" spans="1:2" x14ac:dyDescent="0.2">
@@ -17781,7 +17762,7 @@
         <v>2111</v>
       </c>
       <c r="B2112">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2113" spans="1:2" x14ac:dyDescent="0.2">
@@ -17789,7 +17770,7 @@
         <v>2112</v>
       </c>
       <c r="B2113">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2114" spans="1:2" x14ac:dyDescent="0.2">
@@ -17797,7 +17778,7 @@
         <v>2113</v>
       </c>
       <c r="B2114">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2115" spans="1:2" x14ac:dyDescent="0.2">
@@ -17829,7 +17810,7 @@
         <v>2117</v>
       </c>
       <c r="B2118">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2119" spans="1:2" x14ac:dyDescent="0.2">
@@ -17837,7 +17818,7 @@
         <v>2118</v>
       </c>
       <c r="B2119">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2120" spans="1:2" x14ac:dyDescent="0.2">
@@ -17845,7 +17826,7 @@
         <v>2119</v>
       </c>
       <c r="B2120">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2121" spans="1:2" x14ac:dyDescent="0.2">
@@ -18109,7 +18090,7 @@
         <v>2152</v>
       </c>
       <c r="B2153">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2154" spans="1:2" x14ac:dyDescent="0.2">
@@ -18117,7 +18098,7 @@
         <v>2153</v>
       </c>
       <c r="B2154">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2155" spans="1:2" x14ac:dyDescent="0.2">
@@ -18125,7 +18106,7 @@
         <v>2154</v>
       </c>
       <c r="B2155">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2156" spans="1:2" x14ac:dyDescent="0.2">
@@ -18181,7 +18162,7 @@
         <v>2161</v>
       </c>
       <c r="B2162">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2163" spans="1:2" x14ac:dyDescent="0.2">
@@ -18189,7 +18170,7 @@
         <v>2162</v>
       </c>
       <c r="B2163">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2164" spans="1:2" x14ac:dyDescent="0.2">
@@ -18197,7 +18178,7 @@
         <v>2163</v>
       </c>
       <c r="B2164">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2165" spans="1:2" x14ac:dyDescent="0.2">
@@ -18205,7 +18186,7 @@
         <v>2164</v>
       </c>
       <c r="B2165">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2166" spans="1:2" x14ac:dyDescent="0.2">
@@ -18213,7 +18194,7 @@
         <v>2165</v>
       </c>
       <c r="B2166">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2167" spans="1:2" x14ac:dyDescent="0.2">
@@ -18229,7 +18210,7 @@
         <v>2167</v>
       </c>
       <c r="B2168">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2169" spans="1:2" x14ac:dyDescent="0.2">
@@ -18237,7 +18218,7 @@
         <v>2168</v>
       </c>
       <c r="B2169">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2170" spans="1:2" x14ac:dyDescent="0.2">
@@ -18245,7 +18226,7 @@
         <v>2169</v>
       </c>
       <c r="B2170">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2171" spans="1:2" x14ac:dyDescent="0.2">
@@ -18341,7 +18322,7 @@
         <v>2181</v>
       </c>
       <c r="B2182">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2183" spans="1:2" x14ac:dyDescent="0.2">
@@ -18349,7 +18330,7 @@
         <v>2182</v>
       </c>
       <c r="B2183">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2184" spans="1:2" x14ac:dyDescent="0.2">
@@ -18357,7 +18338,7 @@
         <v>2183</v>
       </c>
       <c r="B2184">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2185" spans="1:2" x14ac:dyDescent="0.2">
@@ -18413,7 +18394,7 @@
         <v>2190</v>
       </c>
       <c r="B2191">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2192" spans="1:2" x14ac:dyDescent="0.2">
@@ -18421,7 +18402,7 @@
         <v>2191</v>
       </c>
       <c r="B2192">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2193" spans="1:2" x14ac:dyDescent="0.2">
@@ -18437,7 +18418,7 @@
         <v>2193</v>
       </c>
       <c r="B2194">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2195" spans="1:2" x14ac:dyDescent="0.2">
@@ -18453,7 +18434,7 @@
         <v>2195</v>
       </c>
       <c r="B2196">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2197" spans="1:2" x14ac:dyDescent="0.2">
@@ -18469,7 +18450,7 @@
         <v>2197</v>
       </c>
       <c r="B2198">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2199" spans="1:2" x14ac:dyDescent="0.2">
@@ -18477,7 +18458,7 @@
         <v>2198</v>
       </c>
       <c r="B2199">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2200" spans="1:2" x14ac:dyDescent="0.2">
@@ -18653,7 +18634,7 @@
         <v>2220</v>
       </c>
       <c r="B2221">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2222" spans="1:2" x14ac:dyDescent="0.2">
@@ -18661,7 +18642,7 @@
         <v>2221</v>
       </c>
       <c r="B2222">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2223" spans="1:2" x14ac:dyDescent="0.2">
@@ -18669,7 +18650,7 @@
         <v>2222</v>
       </c>
       <c r="B2223">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2224" spans="1:2" x14ac:dyDescent="0.2">
@@ -19221,7 +19202,7 @@
         <v>2291</v>
       </c>
       <c r="B2292">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2293" spans="1:2" x14ac:dyDescent="0.2">
@@ -19229,7 +19210,7 @@
         <v>2292</v>
       </c>
       <c r="B2293">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2294" spans="1:2" x14ac:dyDescent="0.2">
@@ -19237,7 +19218,7 @@
         <v>2293</v>
       </c>
       <c r="B2294">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2295" spans="1:2" x14ac:dyDescent="0.2">
@@ -19277,7 +19258,7 @@
         <v>2298</v>
       </c>
       <c r="B2299">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2300" spans="1:2" x14ac:dyDescent="0.2">
@@ -19285,7 +19266,7 @@
         <v>2299</v>
       </c>
       <c r="B2300">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2301" spans="1:2" x14ac:dyDescent="0.2">
@@ -19293,7 +19274,7 @@
         <v>2300</v>
       </c>
       <c r="B2301">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2302" spans="1:2" x14ac:dyDescent="0.2">
@@ -19301,7 +19282,7 @@
         <v>2301</v>
       </c>
       <c r="B2302">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2303" spans="1:2" x14ac:dyDescent="0.2">
@@ -19397,7 +19378,7 @@
         <v>2313</v>
       </c>
       <c r="B2314">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2315" spans="1:2" x14ac:dyDescent="0.2">
@@ -19405,7 +19386,7 @@
         <v>2314</v>
       </c>
       <c r="B2315">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2316" spans="1:2" x14ac:dyDescent="0.2">
@@ -19413,7 +19394,7 @@
         <v>2315</v>
       </c>
       <c r="B2316">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2317" spans="1:2" x14ac:dyDescent="0.2">
@@ -19421,7 +19402,7 @@
         <v>2316</v>
       </c>
       <c r="B2317">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2318" spans="1:2" x14ac:dyDescent="0.2">
@@ -19429,7 +19410,7 @@
         <v>2317</v>
       </c>
       <c r="B2318">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2319" spans="1:2" x14ac:dyDescent="0.2">
@@ -19437,7 +19418,7 @@
         <v>2318</v>
       </c>
       <c r="B2319">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2320" spans="1:2" x14ac:dyDescent="0.2">
@@ -19445,7 +19426,7 @@
         <v>2319</v>
       </c>
       <c r="B2320">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2321" spans="1:2" x14ac:dyDescent="0.2">
@@ -19453,7 +19434,7 @@
         <v>2320</v>
       </c>
       <c r="B2321">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2322" spans="1:2" x14ac:dyDescent="0.2">
@@ -19461,7 +19442,7 @@
         <v>2321</v>
       </c>
       <c r="B2322">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2323" spans="1:2" x14ac:dyDescent="0.2">
@@ -19477,7 +19458,7 @@
         <v>2323</v>
       </c>
       <c r="B2324">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2325" spans="1:2" x14ac:dyDescent="0.2">
@@ -19485,7 +19466,7 @@
         <v>2324</v>
       </c>
       <c r="B2325">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2326" spans="1:2" x14ac:dyDescent="0.2">
@@ -19493,7 +19474,7 @@
         <v>2325</v>
       </c>
       <c r="B2326">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2327" spans="1:2" x14ac:dyDescent="0.2">
@@ -19501,7 +19482,7 @@
         <v>2326</v>
       </c>
       <c r="B2327">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2328" spans="1:2" x14ac:dyDescent="0.2">
@@ -19525,7 +19506,7 @@
         <v>2329</v>
       </c>
       <c r="B2330">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2331" spans="1:2" x14ac:dyDescent="0.2">
@@ -19565,7 +19546,7 @@
         <v>2334</v>
       </c>
       <c r="B2335">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2336" spans="1:2" x14ac:dyDescent="0.2">
@@ -19573,7 +19554,7 @@
         <v>2335</v>
       </c>
       <c r="B2336">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2337" spans="1:2" x14ac:dyDescent="0.2">
@@ -19581,7 +19562,7 @@
         <v>2336</v>
       </c>
       <c r="B2337">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2338" spans="1:2" x14ac:dyDescent="0.2">
@@ -19589,7 +19570,7 @@
         <v>2337</v>
       </c>
       <c r="B2338">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2339" spans="1:2" x14ac:dyDescent="0.2">
@@ -19701,7 +19682,7 @@
         <v>2351</v>
       </c>
       <c r="B2352">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2353" spans="1:2" x14ac:dyDescent="0.2">
@@ -19709,7 +19690,7 @@
         <v>2352</v>
       </c>
       <c r="B2353">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2354" spans="1:2" x14ac:dyDescent="0.2">
@@ -19717,7 +19698,7 @@
         <v>2353</v>
       </c>
       <c r="B2354">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2355" spans="1:2" x14ac:dyDescent="0.2">
@@ -19725,7 +19706,7 @@
         <v>2354</v>
       </c>
       <c r="B2355">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2356" spans="1:2" x14ac:dyDescent="0.2">
@@ -19733,7 +19714,7 @@
         <v>2355</v>
       </c>
       <c r="B2356">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2357" spans="1:2" x14ac:dyDescent="0.2">
@@ -19741,7 +19722,7 @@
         <v>2356</v>
       </c>
       <c r="B2357">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2358" spans="1:2" x14ac:dyDescent="0.2">
@@ -20501,7 +20482,7 @@
         <v>2451</v>
       </c>
       <c r="B2452">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2453" spans="1:2" x14ac:dyDescent="0.2">
@@ -20509,7 +20490,7 @@
         <v>2452</v>
       </c>
       <c r="B2453">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2454" spans="1:2" x14ac:dyDescent="0.2">
@@ -20517,7 +20498,7 @@
         <v>2453</v>
       </c>
       <c r="B2454">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2455" spans="1:2" x14ac:dyDescent="0.2">
@@ -20557,7 +20538,7 @@
         <v>2458</v>
       </c>
       <c r="B2459">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2460" spans="1:2" x14ac:dyDescent="0.2">
@@ -20565,7 +20546,7 @@
         <v>2459</v>
       </c>
       <c r="B2460">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2461" spans="1:2" x14ac:dyDescent="0.2">
@@ -20573,7 +20554,7 @@
         <v>2460</v>
       </c>
       <c r="B2461">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2462" spans="1:2" x14ac:dyDescent="0.2">
@@ -20597,7 +20578,7 @@
         <v>2463</v>
       </c>
       <c r="B2464">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2465" spans="1:2" x14ac:dyDescent="0.2">
@@ -20605,7 +20586,7 @@
         <v>2464</v>
       </c>
       <c r="B2465">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2466" spans="1:2" x14ac:dyDescent="0.2">
@@ -20613,7 +20594,7 @@
         <v>2465</v>
       </c>
       <c r="B2466">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2467" spans="1:2" x14ac:dyDescent="0.2">
@@ -20949,7 +20930,7 @@
         <v>2507</v>
       </c>
       <c r="B2508">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2509" spans="1:2" x14ac:dyDescent="0.2">
@@ -20957,7 +20938,7 @@
         <v>2508</v>
       </c>
       <c r="B2509">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2510" spans="1:2" x14ac:dyDescent="0.2">
@@ -20973,7 +20954,7 @@
         <v>2510</v>
       </c>
       <c r="B2511">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2512" spans="1:2" x14ac:dyDescent="0.2">
@@ -20981,7 +20962,7 @@
         <v>2511</v>
       </c>
       <c r="B2512">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2513" spans="1:2" x14ac:dyDescent="0.2">
@@ -20989,7 +20970,7 @@
         <v>2512</v>
       </c>
       <c r="B2513">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2514" spans="1:2" x14ac:dyDescent="0.2">
@@ -20997,7 +20978,7 @@
         <v>2513</v>
       </c>
       <c r="B2514">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2515" spans="1:2" x14ac:dyDescent="0.2">
@@ -21005,7 +20986,7 @@
         <v>2514</v>
       </c>
       <c r="B2515">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2516" spans="1:2" x14ac:dyDescent="0.2">
@@ -21109,7 +21090,7 @@
         <v>2527</v>
       </c>
       <c r="B2528">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2529" spans="1:2" x14ac:dyDescent="0.2">
@@ -21117,7 +21098,7 @@
         <v>2528</v>
       </c>
       <c r="B2529">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2530" spans="1:2" x14ac:dyDescent="0.2">
@@ -21125,7 +21106,7 @@
         <v>2529</v>
       </c>
       <c r="B2530">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2531" spans="1:2" x14ac:dyDescent="0.2">
@@ -21165,7 +21146,7 @@
         <v>2534</v>
       </c>
       <c r="B2535">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2536" spans="1:2" x14ac:dyDescent="0.2">
@@ -21173,7 +21154,7 @@
         <v>2535</v>
       </c>
       <c r="B2536">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2537" spans="1:2" x14ac:dyDescent="0.2">
@@ -21181,7 +21162,7 @@
         <v>2536</v>
       </c>
       <c r="B2537">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2538" spans="1:2" x14ac:dyDescent="0.2">
@@ -21405,7 +21386,7 @@
         <v>2564</v>
       </c>
       <c r="B2565">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2566" spans="1:2" x14ac:dyDescent="0.2">
@@ -21413,7 +21394,7 @@
         <v>2565</v>
       </c>
       <c r="B2566">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2567" spans="1:2" x14ac:dyDescent="0.2">
@@ -21429,7 +21410,7 @@
         <v>2567</v>
       </c>
       <c r="B2568">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2569" spans="1:2" x14ac:dyDescent="0.2">
@@ -21437,7 +21418,7 @@
         <v>2568</v>
       </c>
       <c r="B2569">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2570" spans="1:2" x14ac:dyDescent="0.2">
@@ -21461,7 +21442,7 @@
         <v>2571</v>
       </c>
       <c r="B2572">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2573" spans="1:2" x14ac:dyDescent="0.2">
@@ -21493,7 +21474,7 @@
         <v>2575</v>
       </c>
       <c r="B2576">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2577" spans="1:2" x14ac:dyDescent="0.2">
@@ -21501,7 +21482,7 @@
         <v>2576</v>
       </c>
       <c r="B2577">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2578" spans="1:2" x14ac:dyDescent="0.2">
@@ -21605,7 +21586,7 @@
         <v>2589</v>
       </c>
       <c r="B2590">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2591" spans="1:2" x14ac:dyDescent="0.2">
@@ -21613,7 +21594,7 @@
         <v>2590</v>
       </c>
       <c r="B2591">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2592" spans="1:2" x14ac:dyDescent="0.2">
@@ -21621,7 +21602,7 @@
         <v>2591</v>
       </c>
       <c r="B2592">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2593" spans="1:2" x14ac:dyDescent="0.2">
@@ -21653,7 +21634,7 @@
         <v>2595</v>
       </c>
       <c r="B2596">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2597" spans="1:2" x14ac:dyDescent="0.2">
@@ -21677,7 +21658,7 @@
         <v>2598</v>
       </c>
       <c r="B2599">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2600" spans="1:2" x14ac:dyDescent="0.2">
@@ -21773,7 +21754,7 @@
         <v>2610</v>
       </c>
       <c r="B2611">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2612" spans="1:2" x14ac:dyDescent="0.2">
@@ -21781,7 +21762,7 @@
         <v>2611</v>
       </c>
       <c r="B2612">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2613" spans="1:2" x14ac:dyDescent="0.2">
@@ -21789,7 +21770,7 @@
         <v>2612</v>
       </c>
       <c r="B2613">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2614" spans="1:2" x14ac:dyDescent="0.2">
@@ -21797,7 +21778,7 @@
         <v>2613</v>
       </c>
       <c r="B2614">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2615" spans="1:2" x14ac:dyDescent="0.2">
@@ -21805,7 +21786,7 @@
         <v>2614</v>
       </c>
       <c r="B2615">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2616" spans="1:2" x14ac:dyDescent="0.2">
@@ -21813,7 +21794,7 @@
         <v>2615</v>
       </c>
       <c r="B2616">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2617" spans="1:2" x14ac:dyDescent="0.2">
@@ -21829,7 +21810,7 @@
         <v>2617</v>
       </c>
       <c r="B2618">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2619" spans="1:2" x14ac:dyDescent="0.2">
@@ -21837,7 +21818,7 @@
         <v>2618</v>
       </c>
       <c r="B2619">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2620" spans="1:2" x14ac:dyDescent="0.2">
@@ -21853,7 +21834,7 @@
         <v>2620</v>
       </c>
       <c r="B2621">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2622" spans="1:2" x14ac:dyDescent="0.2">
@@ -21861,7 +21842,7 @@
         <v>2621</v>
       </c>
       <c r="B2622">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2623" spans="1:2" x14ac:dyDescent="0.2">
@@ -21885,7 +21866,7 @@
         <v>2624</v>
       </c>
       <c r="B2625">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2626" spans="1:2" x14ac:dyDescent="0.2">
@@ -21893,7 +21874,7 @@
         <v>2625</v>
       </c>
       <c r="B2626">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2627" spans="1:2" x14ac:dyDescent="0.2">
@@ -21908,16 +21889,16 @@
       <c r="A2628">
         <v>2627</v>
       </c>
-      <c r="B2628">
-        <v>43</v>
+      <c r="B2628" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2629" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2629">
         <v>2628</v>
       </c>
-      <c r="B2629">
-        <v>61</v>
+      <c r="B2629" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2630" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>